<commit_message>
flujo movimientos cuenta deposito
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaMovimientos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaMovimientos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="48">
   <si>
     <t>ID</t>
   </si>
@@ -93,10 +93,19 @@
     <t>ACTIVO</t>
   </si>
   <si>
-    <t>Cuenta Corriente</t>
+    <t>Corriente</t>
   </si>
   <si>
     <t>406-140100-01</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>creadoosp11</t>
+  </si>
+  <si>
+    <t>406-101530-07</t>
   </si>
   <si>
     <t>Prestamo Personal Ta;Prestamo Personal Ta</t>
@@ -158,10 +167,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -202,7 +211,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -218,12 +227,27 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -232,23 +256,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -277,28 +310,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -306,33 +333,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -365,187 +374,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -577,6 +586,30 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
@@ -585,10 +618,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -605,15 +636,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -635,24 +657,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -674,149 +683,149 @@
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1156,8 +1165,8 @@
   <sheetPr/>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
@@ -1258,19 +1267,49 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
+    <row r="3" spans="1:14">
+      <c r="A3" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="5"/>
@@ -1288,7 +1327,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J2;G3:J3;G4:J4">
       <formula1>Listas!$A$2:$A$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -1399,10 +1438,10 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1464,16 +1503,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1481,50 +1520,50 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>